<commit_message>
a minor edit in trianing trials
</commit_message>
<xml_diff>
--- a/src/omniroute_operation/src/rule_based_experiment/Training_Trials _testing.xlsx
+++ b/src/omniroute_operation/src/rule_based_experiment/Training_Trials _testing.xlsx
@@ -199,10 +199,10 @@
   <dimension ref="A1:G109"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
+      <selection pane="topLeft" activeCell="F52" activeCellId="0" sqref="F52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="11.71"/>
   </cols>
@@ -239,7 +239,7 @@
       </c>
       <c r="E2" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.825916820379567</v>
+        <v>0.921634684664473</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -257,7 +257,7 @@
       </c>
       <c r="E3" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.956715857834677</v>
+        <v>0.85191863093205</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -275,7 +275,7 @@
       </c>
       <c r="E4" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.266402630573717</v>
+        <v>0.633736889328607</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -293,7 +293,7 @@
       </c>
       <c r="E5" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.872875138320842</v>
+        <v>0.401335991315162</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -311,7 +311,7 @@
       </c>
       <c r="E6" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.204235628159313</v>
+        <v>0.750251202111027</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -329,7 +329,7 @@
       </c>
       <c r="E7" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.13926090794488</v>
+        <v>0.929477897708334</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -347,7 +347,7 @@
       </c>
       <c r="E8" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.253588584465513</v>
+        <v>0.755687511656954</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -365,7 +365,7 @@
       </c>
       <c r="E9" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.241168665158558</v>
+        <v>0.769221544645697</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -383,7 +383,7 @@
       </c>
       <c r="E10" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.733290041743077</v>
+        <v>0.596208041834061</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -401,7 +401,7 @@
       </c>
       <c r="E11" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.412438211837976</v>
+        <v>0.2255967613633</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -419,7 +419,7 @@
       </c>
       <c r="E12" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.638721726696423</v>
+        <v>0.951198250464571</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -437,7 +437,7 @@
       </c>
       <c r="E13" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.19632937562536</v>
+        <v>0.0488790568819759</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,7 +455,7 @@
       </c>
       <c r="E14" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.227339909258879</v>
+        <v>0.703670365292586</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -473,7 +473,7 @@
       </c>
       <c r="E15" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.16495777260202</v>
+        <v>0.420475271327699</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -491,7 +491,7 @@
       </c>
       <c r="E16" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.996348928594505</v>
+        <v>0.128427502259809</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -509,7 +509,7 @@
       </c>
       <c r="E17" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.455030680296998</v>
+        <v>0.15428119712782</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -527,7 +527,7 @@
       </c>
       <c r="E18" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.93479742841176</v>
+        <v>0.474129278148238</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -545,7 +545,7 @@
       </c>
       <c r="E19" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.844161639620621</v>
+        <v>0.432320845952754</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -563,7 +563,7 @@
       </c>
       <c r="E20" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.609716875425871</v>
+        <v>0.253267478473597</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -581,7 +581,7 @@
       </c>
       <c r="E21" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.941838726590746</v>
+        <v>0.118673985273208</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -599,7 +599,7 @@
       </c>
       <c r="E22" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.213574871889386</v>
+        <v>0.0308820563246256</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -617,7 +617,7 @@
       </c>
       <c r="E23" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.637824385258543</v>
+        <v>0.862578688329315</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -635,7 +635,7 @@
       </c>
       <c r="E24" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.383624779395707</v>
+        <v>0.195120326831762</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -653,7 +653,7 @@
       </c>
       <c r="E25" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.109163200323352</v>
+        <v>0.314266336549542</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -671,7 +671,7 @@
       </c>
       <c r="E26" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.176189883417813</v>
+        <v>0.629374340731764</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -689,7 +689,7 @@
       </c>
       <c r="E27" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.032308358826401</v>
+        <v>0.852122319403716</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -707,7 +707,7 @@
       </c>
       <c r="E28" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.44581429938578</v>
+        <v>0.765861931194837</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -725,7 +725,7 @@
       </c>
       <c r="E29" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.896267811323078</v>
+        <v>0.850033633686657</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -743,7 +743,7 @@
       </c>
       <c r="E30" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.1059011608131</v>
+        <v>0.315954754787704</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -761,7 +761,7 @@
       </c>
       <c r="E31" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.739687316434034</v>
+        <v>0.334451360526217</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -779,7 +779,7 @@
       </c>
       <c r="E32" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.455710715276725</v>
+        <v>0.358513596246234</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -797,7 +797,7 @@
       </c>
       <c r="E33" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.650143535861105</v>
+        <v>0.655630494054267</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -815,7 +815,7 @@
       </c>
       <c r="E34" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.229973049917661</v>
+        <v>0.931869398810433</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -833,7 +833,7 @@
       </c>
       <c r="E35" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.600326109630079</v>
+        <v>0.796028441239158</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -851,7 +851,7 @@
       </c>
       <c r="E36" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.889028770264648</v>
+        <v>0.222219866056408</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -869,7 +869,7 @@
       </c>
       <c r="E37" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.616620039475744</v>
+        <v>0.104656902230223</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -887,7 +887,7 @@
       </c>
       <c r="E38" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.458161986860549</v>
+        <v>0.549432140646085</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -905,7 +905,7 @@
       </c>
       <c r="E39" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.30582107524279</v>
+        <v>0.470892068807841</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -923,7 +923,7 @@
       </c>
       <c r="E40" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.7576249030918</v>
+        <v>0.607093083292106</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -941,7 +941,7 @@
       </c>
       <c r="E41" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.933497297149158</v>
+        <v>0.792453431987492</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -959,7 +959,7 @@
       </c>
       <c r="E42" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.486186803478871</v>
+        <v>0.262968180667754</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -977,7 +977,7 @@
       </c>
       <c r="E43" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.726786287506788</v>
+        <v>0.361402174020044</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,14 +995,14 @@
       </c>
       <c r="E44" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.640861001828832</v>
+        <v>0.844326272867688</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B45" s="5" t="s">
+      <c r="A45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C45" s="4" t="s">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="E45" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.557416459705858</v>
+        <v>0.214044481442409</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="E46" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.884640933951014</v>
+        <v>0.302703138956899</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="E47" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.477800921025283</v>
+        <v>0.158289598227546</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="E48" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.338145536768248</v>
+        <v>0.816097150398164</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1085,7 +1085,7 @@
       </c>
       <c r="E49" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.511861851638646</v>
+        <v>0.789488486990361</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="E50" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.144831263800444</v>
+        <v>0.292813691819946</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1121,14 +1121,14 @@
       </c>
       <c r="E51" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.504418435336406</v>
+        <v>0.762011620056384</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" s="5" t="s">
+      <c r="A52" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C52" s="4" t="s">
@@ -1139,7 +1139,7 @@
       </c>
       <c r="E52" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.351374754268277</v>
+        <v>0.490145937084936</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1157,7 +1157,7 @@
       </c>
       <c r="E53" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.34062102594694</v>
+        <v>0.881958007409467</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1175,7 +1175,7 @@
       </c>
       <c r="E54" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.402901893992733</v>
+        <v>0.770349749422669</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1193,15 +1193,15 @@
       </c>
       <c r="E55" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.067352011157166</v>
+        <v>0.650242340759133</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>6</v>
+      <c r="B56" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>7</v>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="E56" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.488020842176515</v>
+        <v>0.342787346669932</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="E57" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.241370656936256</v>
+        <v>0.809850275693263</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1247,7 +1247,7 @@
       </c>
       <c r="E58" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.72453523593248</v>
+        <v>0.216933135603902</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1265,7 +1265,7 @@
       </c>
       <c r="E59" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.213846222190663</v>
+        <v>0.452748236237905</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="E60" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.650900516857879</v>
+        <v>0.248473411825707</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="E61" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0263403489227822</v>
+        <v>0.443223123484234</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>